<commit_message>
Update app and CAH project
</commit_message>
<xml_diff>
--- a/scripts/troy/nitrogen_cmpnd_app_tb/data/Compounds_complete.xlsx
+++ b/scripts/troy/nitrogen_cmpnd_app_tb/data/Compounds_complete.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/aed3d806ed7068fe/Documents/GitHub/TARA-thiolases/scripts/troy/nitrogen_cmpnd_app_tb/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="24" documentId="11_EEE3E51FFD43CEAD19E0F8009B4162CC80B470D9" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{9D1A6AA1-AD95-4638-BB59-A4B473CBEC83}"/>
+  <xr:revisionPtr revIDLastSave="26" documentId="11_EEE3E51FFD43CEAD19E0F8009B4162CC80B470D9" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{8ED80BC2-B472-4323-AEE0-5F8738216A55}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="67">
   <si>
     <t>Compound</t>
   </si>
@@ -54,9 +54,6 @@
     <t>C:N Ratio</t>
   </si>
   <si>
-    <t>Cost</t>
-  </si>
-  <si>
     <t>Urea</t>
   </si>
   <si>
@@ -153,9 +150,6 @@
     <t>CAS Reg. 461-58-5</t>
   </si>
   <si>
-    <t>$2,027.50/metric ton</t>
-  </si>
-  <si>
     <t>Methylenediurea</t>
   </si>
   <si>
@@ -183,9 +177,6 @@
     <t>CAS Reg. 2114-02-5</t>
   </si>
   <si>
-    <t>5.20/kg</t>
-  </si>
-  <si>
     <t>www/Allophanate.jpg</t>
   </si>
   <si>
@@ -232,13 +223,19 @@
   </si>
   <si>
     <t>www/Cyanuric_acid.jpg</t>
+  </si>
+  <si>
+    <t>Cost ($/metric ton)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
+  </numFmts>
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -268,6 +265,12 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -283,7 +286,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -291,11 +294,26 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFCCCCCC"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -310,6 +328,13 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="6" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -528,7 +553,7 @@
   <dimension ref="A1:J998"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+      <selection activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.23046875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -539,7 +564,7 @@
     <col min="4" max="26" width="10.53515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -567,238 +592,252 @@
       <c r="I1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="J1" s="9" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A2" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="1" t="s">
+      <c r="B2" s="1" t="s">
         <v>10</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>11</v>
       </c>
       <c r="C2" s="2">
         <v>60.06</v>
       </c>
       <c r="D2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="E2" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="F2" s="1" t="s">
+      <c r="G2" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="H2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="G2" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="H2" s="1" t="s">
+      <c r="I2" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="I2" s="3" t="s">
+      <c r="J2" s="8">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A3" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="1" t="s">
+      <c r="B3" s="1" t="s">
         <v>16</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>17</v>
       </c>
       <c r="C3" s="2">
         <v>103.06</v>
       </c>
       <c r="D3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="F3" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="E3" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="F3" s="4" t="s">
+      <c r="G3" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="H3" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="G3" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="H3" s="1" t="s">
+      <c r="I3" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="I3" s="3" t="s">
+      <c r="J3" s="10"/>
+    </row>
+    <row r="4" spans="1:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A4" s="1" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="1" t="s">
+      <c r="B4" s="1" t="s">
         <v>22</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>23</v>
       </c>
       <c r="C4" s="2">
         <v>42.04</v>
       </c>
       <c r="D4" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="F4" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="E4" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="F4" s="1" t="s">
+      <c r="G4" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="H4" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="G4" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="H4" s="1" t="s">
+      <c r="I4" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="J4" s="8">
+        <v>660</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A5" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="I4" s="3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="1" t="s">
+      <c r="B5" s="1" t="s">
         <v>27</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>28</v>
       </c>
       <c r="C5" s="2">
         <v>103.08</v>
       </c>
       <c r="D5" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="F5" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="E5" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="F5" s="1" t="s">
+      <c r="G5" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="H5" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="G5" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="H5" s="1" t="s">
+      <c r="I5" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="I5" s="3" t="s">
+      <c r="J5" s="8">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A6" s="1" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="1" t="s">
+      <c r="B6" s="1" t="s">
         <v>33</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>34</v>
       </c>
       <c r="C6" s="2">
         <v>129.08000000000001</v>
       </c>
       <c r="D6" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="F6" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="E6" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="F6" s="1" t="s">
+      <c r="G6" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="H6" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="G6" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="H6" s="1" t="s">
+      <c r="I6" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="J6" s="8">
+        <v>990</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A7" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="I6" s="3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="3" t="s">
+      <c r="B7" s="4" t="s">
         <v>38</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>39</v>
       </c>
       <c r="C7" s="5">
         <v>84.08</v>
       </c>
       <c r="D7" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="F7" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="E7" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="F7" s="3" t="s">
+      <c r="G7" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="I7" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="J7" s="8">
+        <v>1540</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A8" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="G7" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="I7" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="J7" s="3" t="s">
+      <c r="B8" s="3" t="s">
         <v>42</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>44</v>
       </c>
       <c r="C8" s="5">
         <v>132.12</v>
       </c>
       <c r="D8" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="G8" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="I8" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="E8" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="F8" s="4" t="s">
+      <c r="J8" s="8">
+        <v>1100</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A9" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="G8" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="I8" s="3" t="s">
+      <c r="B9" s="3" t="s">
         <v>47</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>49</v>
       </c>
       <c r="C9" s="5">
         <v>118.16</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="G9" s="7" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="I9" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="J9" s="3" t="s">
-        <v>52</v>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="J9" s="10"/>
     </row>
     <row r="10" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C10" s="2"/>
@@ -3769,6 +3808,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0" footer="0"/>
-  <pageSetup orientation="landscape"/>
+  <pageSetup orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>